<commit_message>
PCB and BOM updates
Added links to MK_IV bom
Fixed PMOS position and same length USB traces
</commit_message>
<xml_diff>
--- a/-DOCS-/COMPONENTS_LIST/After_Rybnik_BOM.xlsx
+++ b/-DOCS-/COMPONENTS_LIST/After_Rybnik_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\RoboCop\- DOCS -\COMPONENTS LIST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\Sumec-MiniSumo\-DOCS-\COMPONENTS_LIST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367403A2-75A3-4689-9A88-66E9FBE93256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA977A5-9A53-43C5-AD35-470597AAD874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD 1206" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
   <si>
     <t>Footprint</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>10uF, Ceramic</t>
-  </si>
-  <si>
-    <t>6 + 10 doma</t>
   </si>
 </sst>
 </file>
@@ -1275,18 +1272,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37783E8-8A8F-412C-AA35-B13D331D8D66}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:D11"/>
+    <sheetView zoomScale="139" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="3" max="3" width="39.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1298,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1206</v>
       </c>
@@ -1314,7 +1311,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1206</v>
       </c>
@@ -1326,7 +1323,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1206</v>
       </c>
@@ -1339,7 +1336,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1206</v>
       </c>
@@ -1352,7 +1349,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1206</v>
       </c>
@@ -1363,7 +1360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1206</v>
       </c>
@@ -1376,7 +1373,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1206</v>
       </c>
@@ -1390,7 +1387,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1206</v>
       </c>
@@ -1401,7 +1398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1206</v>
       </c>
@@ -1413,7 +1410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1206</v>
       </c>
@@ -1440,20 +1437,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2F9E1B-7F75-4459-928B-AE6722B9CB34}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +1464,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>805</v>
       </c>
@@ -1481,7 +1478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>805</v>
       </c>
@@ -1495,7 +1492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>805</v>
       </c>
@@ -1509,7 +1506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>805</v>
       </c>
@@ -1523,7 +1520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>805</v>
       </c>
@@ -1537,7 +1534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>805</v>
       </c>
@@ -1551,7 +1548,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>805</v>
       </c>
@@ -1562,7 +1559,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>805</v>
       </c>
@@ -1576,7 +1573,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>805</v>
       </c>
@@ -1587,10 +1584,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C13" s="9"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
     </row>
   </sheetData>
@@ -1613,25 +1610,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="53.81640625" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="3" width="45.81640625" customWidth="1"/>
+    <col min="4" max="4" width="57.1796875" customWidth="1"/>
     <col min="5" max="5" width="55" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" customWidth="1"/>
-    <col min="9" max="9" width="34.5703125" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" customWidth="1"/>
+    <col min="8" max="8" width="7.26953125" customWidth="1"/>
+    <col min="9" max="9" width="34.54296875" customWidth="1"/>
+    <col min="10" max="10" width="36.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1646,7 +1643,7 @@
       </c>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1662,7 +1659,7 @@
       <c r="G2" s="1"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1677,7 +1674,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1692,7 +1689,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1707,7 +1704,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1722,7 +1719,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
@@ -1734,7 +1731,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>62</v>
       </c>
@@ -1747,7 +1744,7 @@
       <c r="G8" s="1"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1762,7 +1759,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1777,7 +1774,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1792,7 +1789,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1807,7 +1804,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1822,7 +1819,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -1835,7 +1832,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1850,7 +1847,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1860,12 +1857,12 @@
       <c r="C16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>75</v>
+      <c r="D16" s="1">
+        <v>6</v>
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1878,7 +1875,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -1888,12 +1885,12 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1901,7 +1898,7 @@
       <c r="F20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1909,129 +1906,129 @@
       <c r="F21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="D32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="D36" s="1"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="D37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F46" s="1"/>
     </row>
-    <row r="49" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
       <c r="F52" s="1"/>
     </row>
-    <row r="54" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>

</xml_diff>